<commit_message>
backend completed and its estimation added :fire:
</commit_message>
<xml_diff>
--- a/Estimates.CSV (Challenges).xlsx
+++ b/Estimates.CSV (Challenges).xlsx
@@ -440,10 +440,10 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.31"/>
@@ -715,6 +715,9 @@
       </c>
       <c r="D16" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>1.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>